<commit_message>
subscription sorting and excel uploading
</commit_message>
<xml_diff>
--- a/public/assets/template.xlsx
+++ b/public/assets/template.xlsx
@@ -1,46 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuon\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89DE751C-C3CD-4506-940E-378E6658A01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918ACB4B-DC71-49B4-AE78-7E71DA90DD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23CF16D1-647B-4D17-A8E6-67569E600511}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="3">
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>choice</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>GPTGenerated</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>1 + 1 bang may ?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1 + 2 bang may ?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1 + 3 bang may ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,8 +84,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -66,6 +109,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -93,16 +146,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,59 +474,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A490DE38-7852-400A-AC42-9D7D2A010F29}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>